<commit_message>
added gender to lookup
</commit_message>
<xml_diff>
--- a/question_lookup.xlsx
+++ b/question_lookup.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\johnm\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\johnm\AppData\Local\Temp\scp56140\home\john\research\eclass-public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20305351-437C-452C-A291-3246A431E530}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3EB7DE8-6B07-488F-9501-50684F611108}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22838" yWindow="3728" windowWidth="27524" windowHeight="11422" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1103" yWindow="1103" windowWidth="27525" windowHeight="11422" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="anon_cis" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="anon_post" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">anon_post!$B$26:$C$110</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">anon_post!$B$27:$C$111</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">anon_pre!$A$5:$A$66</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="604" uniqueCount="345">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="607" uniqueCount="348">
   <si>
     <t>Q5</t>
   </si>
@@ -1074,6 +1074,15 @@
   </si>
   <si>
     <t>Other race/ethnicity</t>
+  </si>
+  <si>
+    <t>Q54</t>
+  </si>
+  <si>
+    <t>What is your gender?</t>
+  </si>
+  <si>
+    <t>gender: 1=woman, 2=man, 3=other</t>
   </si>
 </sst>
 </file>
@@ -2525,10 +2534,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6525C988-1BB2-4245-8CC8-092278C926CA}">
-  <dimension ref="A1:DN110"/>
+  <dimension ref="A1:DN111"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -2604,32 +2613,32 @@
     </row>
     <row r="8" spans="1:118">
       <c r="A8" t="s">
-        <v>258</v>
+        <v>345</v>
       </c>
       <c r="B8" t="s">
-        <v>258</v>
+        <v>347</v>
       </c>
       <c r="C8" t="s">
-        <v>308</v>
+        <v>346</v>
       </c>
     </row>
     <row r="9" spans="1:118">
       <c r="A9" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B9" t="s">
-        <v>338</v>
+        <v>258</v>
       </c>
       <c r="C9" t="s">
-        <v>299</v>
+        <v>308</v>
       </c>
     </row>
     <row r="10" spans="1:118">
       <c r="A10" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B10" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="C10" t="s">
         <v>299</v>
@@ -2637,10 +2646,10 @@
     </row>
     <row r="11" spans="1:118">
       <c r="A11" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B11" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="C11" t="s">
         <v>299</v>
@@ -2648,10 +2657,10 @@
     </row>
     <row r="12" spans="1:118">
       <c r="A12" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B12" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="C12" t="s">
         <v>299</v>
@@ -2659,10 +2668,10 @@
     </row>
     <row r="13" spans="1:118">
       <c r="A13" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B13" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="C13" t="s">
         <v>299</v>
@@ -2670,10 +2679,10 @@
     </row>
     <row r="14" spans="1:118">
       <c r="A14" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B14" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="C14" t="s">
         <v>299</v>
@@ -2681,10 +2690,10 @@
     </row>
     <row r="15" spans="1:118">
       <c r="A15" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B15" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="C15" t="s">
         <v>299</v>
@@ -2692,10 +2701,10 @@
     </row>
     <row r="16" spans="1:118">
       <c r="A16" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B16" t="s">
-        <v>1</v>
+        <v>344</v>
       </c>
       <c r="C16" t="s">
         <v>299</v>
@@ -2703,1036 +2712,1047 @@
     </row>
     <row r="17" spans="1:9">
       <c r="A17" t="s">
-        <v>2</v>
+        <v>266</v>
       </c>
       <c r="B17" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C17" t="s">
-        <v>310</v>
+        <v>299</v>
       </c>
     </row>
     <row r="18" spans="1:9">
       <c r="A18" t="s">
-        <v>267</v>
+        <v>2</v>
       </c>
       <c r="B18" t="s">
-        <v>267</v>
+        <v>2</v>
       </c>
       <c r="C18" t="s">
-        <v>307</v>
+        <v>310</v>
       </c>
     </row>
     <row r="19" spans="1:9">
       <c r="A19" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B19" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C19" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
     </row>
     <row r="20" spans="1:9">
       <c r="A20" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B20" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C20" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
     </row>
     <row r="21" spans="1:9">
       <c r="A21" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B21" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C21" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
     </row>
     <row r="22" spans="1:9">
       <c r="A22" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B22" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C22" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
     </row>
     <row r="23" spans="1:9">
       <c r="A23" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B23" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C23" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
     </row>
     <row r="24" spans="1:9">
       <c r="A24" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B24" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="C24" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
     </row>
     <row r="25" spans="1:9">
       <c r="A25" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B25" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C25" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
     </row>
     <row r="26" spans="1:9">
       <c r="A26" t="s">
-        <v>128</v>
+        <v>274</v>
       </c>
       <c r="B26" t="s">
-        <v>128</v>
+        <v>274</v>
       </c>
       <c r="C26" t="s">
-        <v>193</v>
+        <v>300</v>
       </c>
     </row>
     <row r="27" spans="1:9">
       <c r="A27" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B27" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C27" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="28" spans="1:9">
       <c r="A28" t="s">
-        <v>275</v>
+        <v>129</v>
       </c>
       <c r="B28" t="s">
-        <v>275</v>
+        <v>129</v>
       </c>
       <c r="C28" t="s">
-        <v>328</v>
+        <v>194</v>
       </c>
     </row>
     <row r="29" spans="1:9">
       <c r="A29" t="s">
-        <v>150</v>
+        <v>275</v>
       </c>
       <c r="B29" t="s">
-        <v>150</v>
+        <v>275</v>
       </c>
       <c r="C29" t="s">
-        <v>215</v>
-      </c>
-      <c r="I29" s="2"/>
+        <v>328</v>
+      </c>
     </row>
     <row r="30" spans="1:9">
       <c r="A30" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B30" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C30" t="s">
-        <v>216</v>
-      </c>
+        <v>215</v>
+      </c>
+      <c r="I30" s="2"/>
     </row>
     <row r="31" spans="1:9">
       <c r="A31" t="s">
-        <v>276</v>
+        <v>151</v>
       </c>
       <c r="B31" t="s">
-        <v>276</v>
+        <v>151</v>
       </c>
       <c r="C31" t="s">
-        <v>335</v>
+        <v>216</v>
       </c>
     </row>
     <row r="32" spans="1:9">
       <c r="A32" t="s">
-        <v>132</v>
+        <v>276</v>
       </c>
       <c r="B32" t="s">
-        <v>132</v>
+        <v>276</v>
       </c>
       <c r="C32" t="s">
-        <v>197</v>
+        <v>335</v>
       </c>
     </row>
     <row r="33" spans="1:3">
       <c r="A33" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B33" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C33" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="34" spans="1:3">
       <c r="A34" t="s">
-        <v>277</v>
+        <v>133</v>
       </c>
       <c r="B34" t="s">
-        <v>277</v>
+        <v>133</v>
       </c>
       <c r="C34" t="s">
-        <v>320</v>
+        <v>198</v>
       </c>
     </row>
     <row r="35" spans="1:3">
       <c r="A35" t="s">
-        <v>180</v>
+        <v>277</v>
       </c>
       <c r="B35" t="s">
-        <v>180</v>
+        <v>277</v>
       </c>
       <c r="C35" t="s">
-        <v>245</v>
+        <v>320</v>
       </c>
     </row>
     <row r="36" spans="1:3">
       <c r="A36" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B36" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C36" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="37" spans="1:3">
       <c r="A37" t="s">
-        <v>278</v>
+        <v>181</v>
       </c>
       <c r="B37" t="s">
-        <v>278</v>
+        <v>181</v>
       </c>
       <c r="C37" t="s">
-        <v>333</v>
+        <v>246</v>
       </c>
     </row>
     <row r="38" spans="1:3">
       <c r="A38" t="s">
-        <v>146</v>
+        <v>278</v>
       </c>
       <c r="B38" t="s">
-        <v>146</v>
+        <v>278</v>
       </c>
       <c r="C38" t="s">
-        <v>211</v>
+        <v>333</v>
       </c>
     </row>
     <row r="39" spans="1:3">
       <c r="A39" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B39" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C39" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="40" spans="1:3">
       <c r="A40" t="s">
-        <v>279</v>
+        <v>147</v>
       </c>
       <c r="B40" t="s">
-        <v>279</v>
+        <v>147</v>
       </c>
       <c r="C40" t="s">
-        <v>317</v>
+        <v>212</v>
       </c>
     </row>
     <row r="41" spans="1:3">
       <c r="A41" t="s">
-        <v>136</v>
+        <v>279</v>
       </c>
       <c r="B41" t="s">
-        <v>136</v>
+        <v>279</v>
       </c>
       <c r="C41" t="s">
-        <v>201</v>
+        <v>317</v>
       </c>
     </row>
     <row r="42" spans="1:3">
       <c r="A42" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B42" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C42" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="43" spans="1:3">
       <c r="A43" t="s">
-        <v>280</v>
+        <v>137</v>
       </c>
       <c r="B43" t="s">
-        <v>280</v>
+        <v>137</v>
       </c>
       <c r="C43" t="s">
-        <v>330</v>
+        <v>202</v>
       </c>
     </row>
     <row r="44" spans="1:3">
       <c r="A44" t="s">
-        <v>186</v>
+        <v>280</v>
       </c>
       <c r="B44" t="s">
-        <v>186</v>
+        <v>280</v>
       </c>
       <c r="C44" t="s">
-        <v>251</v>
+        <v>330</v>
       </c>
     </row>
     <row r="45" spans="1:3">
       <c r="A45" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B45" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C45" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="46" spans="1:3">
       <c r="A46" t="s">
-        <v>281</v>
+        <v>187</v>
       </c>
       <c r="B46" t="s">
-        <v>281</v>
+        <v>187</v>
       </c>
       <c r="C46" t="s">
-        <v>329</v>
+        <v>252</v>
       </c>
     </row>
     <row r="47" spans="1:3">
       <c r="A47" t="s">
-        <v>168</v>
+        <v>281</v>
       </c>
       <c r="B47" t="s">
-        <v>168</v>
+        <v>281</v>
       </c>
       <c r="C47" t="s">
-        <v>233</v>
+        <v>329</v>
       </c>
     </row>
     <row r="48" spans="1:3">
       <c r="A48" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B48" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C48" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="49" spans="1:3">
       <c r="A49" t="s">
-        <v>282</v>
+        <v>169</v>
       </c>
       <c r="B49" t="s">
-        <v>282</v>
+        <v>169</v>
       </c>
       <c r="C49" t="s">
-        <v>323</v>
+        <v>234</v>
       </c>
     </row>
     <row r="50" spans="1:3">
       <c r="A50" t="s">
-        <v>142</v>
+        <v>282</v>
       </c>
       <c r="B50" t="s">
-        <v>142</v>
+        <v>282</v>
       </c>
       <c r="C50" t="s">
-        <v>207</v>
+        <v>323</v>
       </c>
     </row>
     <row r="51" spans="1:3">
       <c r="A51" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B51" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C51" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="52" spans="1:3">
       <c r="A52" t="s">
-        <v>283</v>
+        <v>143</v>
       </c>
       <c r="B52" t="s">
-        <v>283</v>
+        <v>143</v>
       </c>
       <c r="C52" t="s">
-        <v>327</v>
+        <v>208</v>
       </c>
     </row>
     <row r="53" spans="1:3">
       <c r="A53" t="s">
-        <v>148</v>
+        <v>283</v>
       </c>
       <c r="B53" t="s">
-        <v>148</v>
+        <v>283</v>
       </c>
       <c r="C53" t="s">
-        <v>213</v>
+        <v>327</v>
       </c>
     </row>
     <row r="54" spans="1:3">
       <c r="A54" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B54" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C54" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="55" spans="1:3">
       <c r="A55" t="s">
-        <v>284</v>
+        <v>149</v>
       </c>
       <c r="B55" t="s">
-        <v>284</v>
+        <v>149</v>
       </c>
       <c r="C55" t="s">
-        <v>326</v>
+        <v>214</v>
       </c>
     </row>
     <row r="56" spans="1:3">
       <c r="A56" t="s">
-        <v>174</v>
+        <v>284</v>
       </c>
       <c r="B56" t="s">
-        <v>174</v>
+        <v>284</v>
       </c>
       <c r="C56" t="s">
-        <v>239</v>
+        <v>326</v>
       </c>
     </row>
     <row r="57" spans="1:3">
       <c r="A57" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B57" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C57" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="58" spans="1:3">
       <c r="A58" t="s">
-        <v>285</v>
+        <v>175</v>
       </c>
       <c r="B58" t="s">
-        <v>285</v>
+        <v>175</v>
       </c>
       <c r="C58" t="s">
-        <v>314</v>
+        <v>240</v>
       </c>
     </row>
     <row r="59" spans="1:3">
       <c r="A59" t="s">
-        <v>154</v>
+        <v>285</v>
       </c>
       <c r="B59" t="s">
-        <v>154</v>
+        <v>285</v>
       </c>
       <c r="C59" t="s">
-        <v>219</v>
+        <v>314</v>
       </c>
     </row>
     <row r="60" spans="1:3">
       <c r="A60" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B60" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C60" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="61" spans="1:3">
       <c r="A61" t="s">
-        <v>286</v>
+        <v>155</v>
       </c>
       <c r="B61" t="s">
-        <v>286</v>
+        <v>155</v>
       </c>
       <c r="C61" t="s">
-        <v>325</v>
+        <v>220</v>
       </c>
     </row>
     <row r="62" spans="1:3">
       <c r="A62" t="s">
-        <v>182</v>
+        <v>286</v>
       </c>
       <c r="B62" t="s">
-        <v>182</v>
+        <v>286</v>
       </c>
       <c r="C62" t="s">
-        <v>247</v>
+        <v>325</v>
       </c>
     </row>
     <row r="63" spans="1:3">
       <c r="A63" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B63" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C63" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="64" spans="1:3">
       <c r="A64" t="s">
-        <v>287</v>
+        <v>183</v>
       </c>
       <c r="B64" t="s">
-        <v>287</v>
+        <v>183</v>
       </c>
       <c r="C64" t="s">
-        <v>319</v>
+        <v>248</v>
       </c>
     </row>
     <row r="65" spans="1:3">
       <c r="A65" t="s">
-        <v>156</v>
+        <v>287</v>
       </c>
       <c r="B65" t="s">
-        <v>156</v>
+        <v>287</v>
       </c>
       <c r="C65" t="s">
-        <v>221</v>
+        <v>319</v>
       </c>
     </row>
     <row r="66" spans="1:3">
       <c r="A66" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B66" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C66" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="67" spans="1:3">
       <c r="A67" t="s">
-        <v>288</v>
+        <v>157</v>
       </c>
       <c r="B67" t="s">
-        <v>288</v>
+        <v>157</v>
       </c>
       <c r="C67" t="s">
-        <v>324</v>
+        <v>222</v>
       </c>
     </row>
     <row r="68" spans="1:3">
       <c r="A68" t="s">
-        <v>160</v>
+        <v>288</v>
       </c>
       <c r="B68" t="s">
-        <v>160</v>
+        <v>288</v>
       </c>
       <c r="C68" t="s">
-        <v>225</v>
+        <v>324</v>
       </c>
     </row>
     <row r="69" spans="1:3">
       <c r="A69" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B69" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C69" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="70" spans="1:3">
       <c r="A70" t="s">
-        <v>289</v>
+        <v>161</v>
       </c>
       <c r="B70" t="s">
-        <v>289</v>
+        <v>161</v>
       </c>
       <c r="C70" t="s">
-        <v>322</v>
+        <v>226</v>
       </c>
     </row>
     <row r="71" spans="1:3">
       <c r="A71" t="s">
-        <v>178</v>
+        <v>289</v>
       </c>
       <c r="B71" t="s">
-        <v>178</v>
+        <v>289</v>
       </c>
       <c r="C71" t="s">
-        <v>243</v>
+        <v>322</v>
       </c>
     </row>
     <row r="72" spans="1:3">
       <c r="A72" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B72" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C72" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="73" spans="1:3">
       <c r="A73" t="s">
-        <v>290</v>
+        <v>179</v>
       </c>
       <c r="B73" t="s">
-        <v>290</v>
+        <v>179</v>
       </c>
       <c r="C73" t="s">
-        <v>331</v>
+        <v>244</v>
       </c>
     </row>
     <row r="74" spans="1:3">
       <c r="A74" t="s">
-        <v>162</v>
+        <v>290</v>
       </c>
       <c r="B74" t="s">
-        <v>162</v>
+        <v>290</v>
       </c>
       <c r="C74" t="s">
-        <v>227</v>
+        <v>331</v>
       </c>
     </row>
     <row r="75" spans="1:3">
       <c r="A75" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B75" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C75" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="76" spans="1:3">
       <c r="A76" t="s">
-        <v>291</v>
+        <v>163</v>
       </c>
       <c r="B76" t="s">
-        <v>291</v>
+        <v>163</v>
       </c>
       <c r="C76" t="s">
-        <v>321</v>
+        <v>228</v>
       </c>
     </row>
     <row r="77" spans="1:3">
       <c r="A77" t="s">
-        <v>138</v>
+        <v>291</v>
       </c>
       <c r="B77" t="s">
-        <v>138</v>
+        <v>291</v>
       </c>
       <c r="C77" t="s">
-        <v>203</v>
+        <v>321</v>
       </c>
     </row>
     <row r="78" spans="1:3">
       <c r="A78" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B78" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C78" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="79" spans="1:3">
       <c r="A79" t="s">
-        <v>292</v>
+        <v>139</v>
       </c>
       <c r="B79" t="s">
-        <v>292</v>
+        <v>139</v>
       </c>
       <c r="C79" t="s">
-        <v>334</v>
+        <v>204</v>
       </c>
     </row>
     <row r="80" spans="1:3">
       <c r="A80" t="s">
-        <v>164</v>
+        <v>292</v>
       </c>
       <c r="B80" t="s">
-        <v>164</v>
+        <v>292</v>
       </c>
       <c r="C80" t="s">
-        <v>229</v>
+        <v>334</v>
       </c>
     </row>
     <row r="81" spans="1:3">
       <c r="A81" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B81" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C81" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="82" spans="1:3">
       <c r="A82" t="s">
-        <v>293</v>
+        <v>165</v>
       </c>
       <c r="B82" t="s">
-        <v>293</v>
+        <v>165</v>
       </c>
       <c r="C82" t="s">
-        <v>332</v>
+        <v>230</v>
       </c>
     </row>
     <row r="83" spans="1:3">
       <c r="A83" t="s">
-        <v>170</v>
+        <v>293</v>
       </c>
       <c r="B83" t="s">
-        <v>170</v>
+        <v>293</v>
       </c>
       <c r="C83" t="s">
-        <v>235</v>
+        <v>332</v>
       </c>
     </row>
     <row r="84" spans="1:3">
       <c r="A84" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B84" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C84" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="85" spans="1:3">
       <c r="A85" t="s">
-        <v>294</v>
+        <v>171</v>
       </c>
       <c r="B85" t="s">
-        <v>294</v>
+        <v>171</v>
       </c>
       <c r="C85" t="s">
-        <v>318</v>
+        <v>236</v>
       </c>
     </row>
     <row r="86" spans="1:3">
       <c r="A86" t="s">
-        <v>134</v>
+        <v>294</v>
       </c>
       <c r="B86" t="s">
-        <v>134</v>
+        <v>294</v>
       </c>
       <c r="C86" t="s">
-        <v>199</v>
+        <v>318</v>
       </c>
     </row>
     <row r="87" spans="1:3">
       <c r="A87" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B87" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C87" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="88" spans="1:3">
       <c r="A88" t="s">
-        <v>295</v>
+        <v>135</v>
       </c>
       <c r="B88" t="s">
-        <v>295</v>
+        <v>135</v>
       </c>
       <c r="C88" t="s">
-        <v>316</v>
+        <v>200</v>
       </c>
     </row>
     <row r="89" spans="1:3">
       <c r="A89" t="s">
-        <v>166</v>
+        <v>295</v>
       </c>
       <c r="B89" t="s">
-        <v>166</v>
+        <v>295</v>
       </c>
       <c r="C89" t="s">
-        <v>231</v>
+        <v>316</v>
       </c>
     </row>
     <row r="90" spans="1:3">
       <c r="A90" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B90" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C90" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="91" spans="1:3">
       <c r="A91" t="s">
-        <v>140</v>
+        <v>167</v>
       </c>
       <c r="B91" t="s">
-        <v>140</v>
+        <v>167</v>
       </c>
       <c r="C91" t="s">
-        <v>205</v>
+        <v>232</v>
       </c>
     </row>
     <row r="92" spans="1:3">
       <c r="A92" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B92" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C92" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="93" spans="1:3">
       <c r="A93" t="s">
-        <v>176</v>
+        <v>141</v>
       </c>
       <c r="B93" t="s">
-        <v>176</v>
+        <v>141</v>
       </c>
       <c r="C93" t="s">
-        <v>241</v>
+        <v>206</v>
       </c>
     </row>
     <row r="94" spans="1:3">
       <c r="A94" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B94" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C94" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="95" spans="1:3">
       <c r="A95" t="s">
-        <v>152</v>
+        <v>177</v>
       </c>
       <c r="B95" t="s">
-        <v>152</v>
+        <v>177</v>
       </c>
       <c r="C95" t="s">
-        <v>217</v>
+        <v>242</v>
       </c>
     </row>
     <row r="96" spans="1:3">
       <c r="A96" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B96" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C96" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="97" spans="1:3">
       <c r="A97" t="s">
-        <v>130</v>
+        <v>153</v>
       </c>
       <c r="B97" t="s">
-        <v>130</v>
+        <v>153</v>
       </c>
       <c r="C97" t="s">
-        <v>195</v>
+        <v>218</v>
       </c>
     </row>
     <row r="98" spans="1:3">
       <c r="A98" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B98" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C98" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="99" spans="1:3">
       <c r="A99" t="s">
-        <v>144</v>
+        <v>131</v>
       </c>
       <c r="B99" t="s">
-        <v>144</v>
+        <v>131</v>
       </c>
       <c r="C99" t="s">
-        <v>209</v>
+        <v>196</v>
       </c>
     </row>
     <row r="100" spans="1:3">
       <c r="A100" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B100" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C100" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="101" spans="1:3">
       <c r="A101" t="s">
-        <v>296</v>
+        <v>145</v>
       </c>
       <c r="B101" t="s">
-        <v>296</v>
+        <v>145</v>
       </c>
       <c r="C101" t="s">
-        <v>315</v>
+        <v>210</v>
       </c>
     </row>
     <row r="102" spans="1:3">
       <c r="A102" t="s">
-        <v>184</v>
+        <v>296</v>
       </c>
       <c r="B102" t="s">
-        <v>184</v>
+        <v>296</v>
       </c>
       <c r="C102" t="s">
-        <v>249</v>
+        <v>315</v>
       </c>
     </row>
     <row r="103" spans="1:3">
       <c r="A103" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B103" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C103" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="104" spans="1:3">
       <c r="A104" t="s">
-        <v>158</v>
+        <v>185</v>
       </c>
       <c r="B104" t="s">
-        <v>158</v>
+        <v>185</v>
       </c>
       <c r="C104" t="s">
-        <v>223</v>
+        <v>250</v>
       </c>
     </row>
     <row r="105" spans="1:3">
       <c r="A105" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B105" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C105" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="106" spans="1:3">
       <c r="A106" t="s">
-        <v>297</v>
+        <v>159</v>
       </c>
       <c r="B106" t="s">
-        <v>297</v>
+        <v>159</v>
       </c>
       <c r="C106" t="s">
-        <v>313</v>
+        <v>224</v>
       </c>
     </row>
     <row r="107" spans="1:3">
       <c r="A107" t="s">
-        <v>188</v>
+        <v>297</v>
       </c>
       <c r="B107" t="s">
-        <v>188</v>
+        <v>297</v>
       </c>
       <c r="C107" t="s">
-        <v>253</v>
+        <v>313</v>
       </c>
     </row>
     <row r="108" spans="1:3">
       <c r="A108" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B108" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C108" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="109" spans="1:3">
       <c r="A109" t="s">
-        <v>172</v>
+        <v>189</v>
       </c>
       <c r="B109" t="s">
-        <v>172</v>
+        <v>189</v>
       </c>
       <c r="C109" t="s">
-        <v>337</v>
+        <v>254</v>
       </c>
     </row>
     <row r="110" spans="1:3">
       <c r="A110" t="s">
+        <v>172</v>
+      </c>
+      <c r="B110" t="s">
+        <v>172</v>
+      </c>
+      <c r="C110" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3">
+      <c r="A111" t="s">
         <v>173</v>
       </c>
-      <c r="B110" t="s">
+      <c r="B111" t="s">
         <v>173</v>
       </c>
-      <c r="C110" t="s">
+      <c r="C111" t="s">
         <v>336</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added responseid to survey lookup spreadsheet
</commit_message>
<xml_diff>
--- a/question_lookup.xlsx
+++ b/question_lookup.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\johnm\AppData\Local\Temp\scp56140\home\john\research\eclass-public\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\johnm\AppData\Local\Temp\scp23002\home\john\research\eclass-public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3EB7DE8-6B07-488F-9501-50684F611108}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2EA7C3D-DA3A-4E20-9FC3-2EF451620973}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1103" yWindow="1103" windowWidth="27525" windowHeight="11422" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1103" yWindow="1103" windowWidth="27525" windowHeight="11422" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="anon_cis" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="607" uniqueCount="348">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="611" uniqueCount="349">
   <si>
     <t>Q5</t>
   </si>
@@ -1083,6 +1083,9 @@
   </si>
   <si>
     <t>gender: 1=woman, 2=man, 3=other</t>
+  </si>
+  <si>
+    <t>A unique ID for the survey for both pre and post</t>
   </si>
 </sst>
 </file>
@@ -1984,10 +1987,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D80AE906-8B18-4E75-B911-7516D9D2B196}">
-  <dimension ref="A1:C66"/>
+  <dimension ref="A1:C67"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B4"/>
+    <sheetView tabSelected="1" topLeftCell="A50" workbookViewId="0">
+      <selection activeCell="A67" sqref="A67:B67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -2527,6 +2530,14 @@
         <v>254</v>
       </c>
     </row>
+    <row r="67" spans="1:3">
+      <c r="A67" t="s">
+        <v>46</v>
+      </c>
+      <c r="B67" t="s">
+        <v>348</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2534,10 +2545,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6525C988-1BB2-4245-8CC8-092278C926CA}">
-  <dimension ref="A1:DN111"/>
+  <dimension ref="A1:DN112"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView topLeftCell="A104" workbookViewId="0">
+      <selection activeCell="A112" sqref="A112:B112"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -3756,6 +3767,14 @@
         <v>336</v>
       </c>
     </row>
+    <row r="112" spans="1:3">
+      <c r="A112" t="s">
+        <v>46</v>
+      </c>
+      <c r="B112" t="s">
+        <v>348</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
created buffy v intro notebook added details to metadata table
</commit_message>
<xml_diff>
--- a/question_lookup.xlsx
+++ b/question_lookup.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22827"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\johnm\AppData\Local\Temp\scp23002\home\john\research\eclass-public\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\John\AppData\Local\Temp\scp01687\home\john\research\eclass-public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2EA7C3D-DA3A-4E20-9FC3-2EF451620973}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1103" yWindow="1103" windowWidth="27525" windowHeight="11422" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1110" yWindow="1110" windowWidth="27525" windowHeight="11415" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="anon_cis" sheetId="1" r:id="rId1"/>
@@ -31,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="611" uniqueCount="349">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="611" uniqueCount="357">
   <si>
     <t>Q5</t>
   </si>
@@ -1086,12 +1085,36 @@
   </si>
   <si>
     <t>A unique ID for the survey for both pre and post</t>
+  </si>
+  <si>
+    <t>Q53_1, yes=1; no=2</t>
+  </si>
+  <si>
+    <t>Q53_2, yes=1; no=2</t>
+  </si>
+  <si>
+    <t>Q53_3, yes=1; no=2</t>
+  </si>
+  <si>
+    <t>Q53_4, yes=1; no=2</t>
+  </si>
+  <si>
+    <t>Q53_5, yes=1; no=2</t>
+  </si>
+  <si>
+    <t>Q53_6, yes=1; no=2</t>
+  </si>
+  <si>
+    <t>Q53_7, yes=1; no=2</t>
+  </si>
+  <si>
+    <t>Q53_8, yes=1; no=2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="4">
     <font>
       <sz val="11"/>
@@ -1434,18 +1457,18 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C50"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B51" sqref="B51"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="15.73046875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="29.265625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="49.33203125" style="2" customWidth="1"/>
+    <col min="1" max="1" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.28515625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="49.28515625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -1459,7 +1482,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" ht="30">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1470,7 +1493,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="28.5">
+    <row r="3" spans="1:3" ht="30">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -1481,7 +1504,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="28.5">
+    <row r="4" spans="1:3" ht="30">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -1492,7 +1515,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="71.25">
+    <row r="5" spans="1:3" ht="90">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -1503,7 +1526,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" ht="30">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -1514,7 +1537,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="42.75">
+    <row r="7" spans="1:3" ht="60">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -1525,7 +1548,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="28.5">
+    <row r="8" spans="1:3" ht="45">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -1536,7 +1559,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="28.5">
+    <row r="9" spans="1:3" ht="30">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -1558,7 +1581,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="42.75">
+    <row r="11" spans="1:3" ht="60">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -1580,7 +1603,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="71.25">
+    <row r="13" spans="1:3" ht="90">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -1591,7 +1614,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="71.25">
+    <row r="14" spans="1:3" ht="90">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -1602,7 +1625,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:3" ht="30">
       <c r="A15" t="s">
         <v>13</v>
       </c>
@@ -1613,7 +1636,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="57">
+    <row r="16" spans="1:3" ht="60">
       <c r="A16" t="s">
         <v>14</v>
       </c>
@@ -1635,7 +1658,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="85.5">
+    <row r="18" spans="1:3" ht="90">
       <c r="A18" t="s">
         <v>16</v>
       </c>
@@ -1646,7 +1669,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="85.5">
+    <row r="19" spans="1:3" ht="90">
       <c r="A19" t="s">
         <v>17</v>
       </c>
@@ -1657,7 +1680,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="85.5">
+    <row r="20" spans="1:3" ht="90">
       <c r="A20" t="s">
         <v>18</v>
       </c>
@@ -1956,7 +1979,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="48" spans="1:3" ht="28.5">
+    <row r="48" spans="1:3" ht="30">
       <c r="A48" t="s">
         <v>46</v>
       </c>
@@ -1964,7 +1987,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="49" spans="1:2" ht="28.5">
+    <row r="49" spans="1:2" ht="30">
       <c r="A49" t="s">
         <v>47</v>
       </c>
@@ -1972,7 +1995,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="50" spans="1:2" ht="28.5">
+    <row r="50" spans="1:2" ht="30">
       <c r="A50" t="s">
         <v>48</v>
       </c>
@@ -1986,17 +2009,17 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D80AE906-8B18-4E75-B911-7516D9D2B196}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A50" workbookViewId="0">
+    <sheetView topLeftCell="A38" workbookViewId="0">
       <selection activeCell="A67" sqref="A67:B67"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="14.19921875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" s="1" customFormat="1">
@@ -2544,14 +2567,17 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6525C988-1BB2-4245-8CC8-092278C926CA}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:DN112"/>
   <sheetViews>
-    <sheetView topLeftCell="A104" workbookViewId="0">
-      <selection activeCell="A112" sqref="A112:B112"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="53.28515625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:118">
       <c r="A1" s="1" t="s">
@@ -2748,7 +2774,7 @@
         <v>267</v>
       </c>
       <c r="B19" t="s">
-        <v>267</v>
+        <v>349</v>
       </c>
       <c r="C19" t="s">
         <v>307</v>
@@ -2759,7 +2785,7 @@
         <v>268</v>
       </c>
       <c r="B20" t="s">
-        <v>268</v>
+        <v>350</v>
       </c>
       <c r="C20" t="s">
         <v>306</v>
@@ -2770,7 +2796,7 @@
         <v>269</v>
       </c>
       <c r="B21" t="s">
-        <v>269</v>
+        <v>351</v>
       </c>
       <c r="C21" t="s">
         <v>305</v>
@@ -2781,7 +2807,7 @@
         <v>270</v>
       </c>
       <c r="B22" t="s">
-        <v>270</v>
+        <v>352</v>
       </c>
       <c r="C22" t="s">
         <v>304</v>
@@ -2792,7 +2818,7 @@
         <v>271</v>
       </c>
       <c r="B23" t="s">
-        <v>271</v>
+        <v>353</v>
       </c>
       <c r="C23" t="s">
         <v>303</v>
@@ -2803,7 +2829,7 @@
         <v>272</v>
       </c>
       <c r="B24" t="s">
-        <v>272</v>
+        <v>354</v>
       </c>
       <c r="C24" t="s">
         <v>302</v>
@@ -2814,7 +2840,7 @@
         <v>273</v>
       </c>
       <c r="B25" t="s">
-        <v>273</v>
+        <v>355</v>
       </c>
       <c r="C25" t="s">
         <v>301</v>
@@ -2825,7 +2851,7 @@
         <v>274</v>
       </c>
       <c r="B26" t="s">
-        <v>274</v>
+        <v>356</v>
       </c>
       <c r="C26" t="s">
         <v>300</v>

</xml_diff>

<commit_message>
Updated question_lookup to include information about majors. Added optional 'route' variable to DataHelper.py.
</commit_message>
<xml_diff>
--- a/question_lookup.xlsx
+++ b/question_lookup.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11213"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\John\AppData\Local\Temp\scp01687\home\john\research\eclass-public\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fox/Google Drive/Boulder/PER/ECLASS/eclass-public/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{212EDCAB-AD8D-2544-B1D8-4D0233B93AEC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1110" yWindow="1110" windowWidth="27525" windowHeight="11415" activeTab="2"/>
+    <workbookView xWindow="1120" yWindow="1120" windowWidth="27520" windowHeight="11420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="anon_cis" sheetId="1" r:id="rId1"/>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="611" uniqueCount="357">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="611" uniqueCount="358">
   <si>
     <t>Q5</t>
   </si>
@@ -1109,13 +1110,16 @@
   </si>
   <si>
     <t>Q53_8, yes=1; no=2</t>
+  </si>
+  <si>
+    <t>Q47: 1 = Physics, 2 = Chemistry, 3 = Biochemistry, 4 = Biology, 5 = Engineering, 6 = Engineering Physics, 7 = Astronomy, 8 = Astrophysics, 9 = Geology/Geophysics, 10 = Math/Applied Math, 11 = Computer Science, 12 = Physiology, 13 = Other science, 14 = Non-science major, 15 = Open Option/undeclared.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1457,21 +1461,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C50"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B51" sqref="B51"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="29.28515625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="49.28515625" style="2" customWidth="1"/>
+    <col min="1" max="1" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.33203125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="49.33203125" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>49</v>
       </c>
@@ -1482,7 +1486,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="30">
+    <row r="2" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1493,7 +1497,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="30">
+    <row r="3" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -1504,7 +1508,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="30">
+    <row r="4" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -1515,7 +1519,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="90">
+    <row r="5" spans="1:3" ht="80" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -1526,7 +1530,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="30">
+    <row r="6" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -1537,7 +1541,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="60">
+    <row r="7" spans="1:3" ht="48" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -1548,7 +1552,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="45">
+    <row r="8" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -1559,7 +1563,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="30">
+    <row r="9" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -1570,7 +1574,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -1581,7 +1585,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="60">
+    <row r="11" spans="1:3" ht="48" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -1592,7 +1596,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -1603,7 +1607,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="90">
+    <row r="13" spans="1:3" ht="80" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -1614,7 +1618,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="90">
+    <row r="14" spans="1:3" ht="80" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -1625,7 +1629,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="30">
+    <row r="15" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>13</v>
       </c>
@@ -1636,7 +1640,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="60">
+    <row r="16" spans="1:3" ht="64" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>14</v>
       </c>
@@ -1647,7 +1651,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>15</v>
       </c>
@@ -1658,7 +1662,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="90">
+    <row r="18" spans="1:3" ht="96" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>16</v>
       </c>
@@ -1669,7 +1673,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="90">
+    <row r="19" spans="1:3" ht="96" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>17</v>
       </c>
@@ -1680,7 +1684,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="90">
+    <row r="20" spans="1:3" ht="96" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>18</v>
       </c>
@@ -1691,7 +1695,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="21" spans="1:3">
+    <row r="21" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>19</v>
       </c>
@@ -1702,7 +1706,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="22" spans="1:3">
+    <row r="22" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>20</v>
       </c>
@@ -1713,7 +1717,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="23" spans="1:3">
+    <row r="23" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>21</v>
       </c>
@@ -1724,7 +1728,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="24" spans="1:3">
+    <row r="24" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>22</v>
       </c>
@@ -1735,7 +1739,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="25" spans="1:3">
+    <row r="25" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>23</v>
       </c>
@@ -1746,7 +1750,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="26" spans="1:3">
+    <row r="26" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>24</v>
       </c>
@@ -1757,7 +1761,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="27" spans="1:3">
+    <row r="27" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>25</v>
       </c>
@@ -1768,7 +1772,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="28" spans="1:3">
+    <row r="28" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>26</v>
       </c>
@@ -1779,7 +1783,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="29" spans="1:3">
+    <row r="29" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>27</v>
       </c>
@@ -1790,7 +1794,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="30" spans="1:3">
+    <row r="30" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>28</v>
       </c>
@@ -1801,7 +1805,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="31" spans="1:3">
+    <row r="31" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>29</v>
       </c>
@@ -1812,7 +1816,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="32" spans="1:3">
+    <row r="32" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>30</v>
       </c>
@@ -1823,7 +1827,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="33" spans="1:3">
+    <row r="33" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>31</v>
       </c>
@@ -1834,7 +1838,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="34" spans="1:3">
+    <row r="34" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>32</v>
       </c>
@@ -1845,7 +1849,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="35" spans="1:3">
+    <row r="35" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>33</v>
       </c>
@@ -1856,7 +1860,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="36" spans="1:3">
+    <row r="36" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>34</v>
       </c>
@@ -1867,7 +1871,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="37" spans="1:3">
+    <row r="37" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>35</v>
       </c>
@@ -1878,7 +1882,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="38" spans="1:3">
+    <row r="38" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>36</v>
       </c>
@@ -1889,7 +1893,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="39" spans="1:3">
+    <row r="39" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>37</v>
       </c>
@@ -1900,7 +1904,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="40" spans="1:3">
+    <row r="40" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>38</v>
       </c>
@@ -1911,7 +1915,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="41" spans="1:3">
+    <row r="41" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>39</v>
       </c>
@@ -1922,7 +1926,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="42" spans="1:3">
+    <row r="42" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>40</v>
       </c>
@@ -1933,7 +1937,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="43" spans="1:3">
+    <row r="43" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>41</v>
       </c>
@@ -1944,7 +1948,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="44" spans="1:3">
+    <row r="44" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>42</v>
       </c>
@@ -1955,7 +1959,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="45" spans="1:3">
+    <row r="45" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>43</v>
       </c>
@@ -1963,7 +1967,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="46" spans="1:3">
+    <row r="46" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>44</v>
       </c>
@@ -1971,7 +1975,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="47" spans="1:3">
+    <row r="47" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>45</v>
       </c>
@@ -1979,7 +1983,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="48" spans="1:3" ht="30">
+    <row r="48" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>46</v>
       </c>
@@ -1987,7 +1991,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="49" spans="1:2" ht="30">
+    <row r="49" spans="1:2" ht="32" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>47</v>
       </c>
@@ -1995,7 +1999,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="50" spans="1:2" ht="30">
+    <row r="50" spans="1:2" ht="32" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>48</v>
       </c>
@@ -2009,20 +2013,20 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C67"/>
   <sheetViews>
     <sheetView topLeftCell="A38" workbookViewId="0">
       <selection activeCell="A67" sqref="A67:B67"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="1" customFormat="1">
+    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>49</v>
       </c>
@@ -2033,7 +2037,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
         <v>125</v>
       </c>
@@ -2041,7 +2045,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>126</v>
       </c>
@@ -2049,7 +2053,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>127</v>
       </c>
@@ -2057,7 +2061,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>128</v>
       </c>
@@ -2065,7 +2069,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>129</v>
       </c>
@@ -2073,7 +2077,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>130</v>
       </c>
@@ -2081,7 +2085,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>131</v>
       </c>
@@ -2089,7 +2093,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>132</v>
       </c>
@@ -2097,7 +2101,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>133</v>
       </c>
@@ -2105,7 +2109,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>134</v>
       </c>
@@ -2113,7 +2117,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>135</v>
       </c>
@@ -2121,7 +2125,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>136</v>
       </c>
@@ -2129,7 +2133,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>137</v>
       </c>
@@ -2137,7 +2141,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>138</v>
       </c>
@@ -2145,7 +2149,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="16" spans="1:3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>139</v>
       </c>
@@ -2153,7 +2157,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>140</v>
       </c>
@@ -2161,7 +2165,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="18" spans="1:3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>141</v>
       </c>
@@ -2169,7 +2173,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="19" spans="1:3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>142</v>
       </c>
@@ -2177,7 +2181,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="20" spans="1:3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>143</v>
       </c>
@@ -2185,7 +2189,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="21" spans="1:3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>144</v>
       </c>
@@ -2193,7 +2197,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="22" spans="1:3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>145</v>
       </c>
@@ -2201,7 +2205,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="23" spans="1:3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>146</v>
       </c>
@@ -2209,7 +2213,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="24" spans="1:3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>147</v>
       </c>
@@ -2217,7 +2221,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="25" spans="1:3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>148</v>
       </c>
@@ -2225,7 +2229,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="26" spans="1:3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>149</v>
       </c>
@@ -2233,7 +2237,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="27" spans="1:3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>150</v>
       </c>
@@ -2241,7 +2245,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="28" spans="1:3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>151</v>
       </c>
@@ -2249,7 +2253,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="29" spans="1:3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>152</v>
       </c>
@@ -2257,7 +2261,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="30" spans="1:3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>153</v>
       </c>
@@ -2265,7 +2269,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="31" spans="1:3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>154</v>
       </c>
@@ -2273,7 +2277,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="32" spans="1:3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>155</v>
       </c>
@@ -2281,7 +2285,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="33" spans="1:3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>156</v>
       </c>
@@ -2289,7 +2293,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="34" spans="1:3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>157</v>
       </c>
@@ -2297,7 +2301,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="35" spans="1:3">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>158</v>
       </c>
@@ -2305,7 +2309,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="36" spans="1:3">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>159</v>
       </c>
@@ -2313,7 +2317,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="37" spans="1:3">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>160</v>
       </c>
@@ -2321,7 +2325,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="38" spans="1:3">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>161</v>
       </c>
@@ -2329,7 +2333,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="39" spans="1:3">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>162</v>
       </c>
@@ -2337,7 +2341,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="40" spans="1:3">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>163</v>
       </c>
@@ -2345,7 +2349,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="41" spans="1:3">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>164</v>
       </c>
@@ -2353,7 +2357,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="42" spans="1:3">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>165</v>
       </c>
@@ -2361,7 +2365,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="43" spans="1:3">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>166</v>
       </c>
@@ -2369,7 +2373,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="44" spans="1:3">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>167</v>
       </c>
@@ -2377,7 +2381,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="45" spans="1:3">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>168</v>
       </c>
@@ -2385,7 +2389,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="46" spans="1:3">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>169</v>
       </c>
@@ -2393,7 +2397,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="47" spans="1:3">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>170</v>
       </c>
@@ -2401,7 +2405,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="48" spans="1:3">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>171</v>
       </c>
@@ -2409,7 +2413,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="49" spans="1:3">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>172</v>
       </c>
@@ -2417,7 +2421,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="50" spans="1:3">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>173</v>
       </c>
@@ -2425,7 +2429,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="51" spans="1:3">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>174</v>
       </c>
@@ -2433,7 +2437,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="52" spans="1:3">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>175</v>
       </c>
@@ -2441,7 +2445,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="53" spans="1:3">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>176</v>
       </c>
@@ -2449,7 +2453,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="54" spans="1:3">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>177</v>
       </c>
@@ -2457,7 +2461,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="55" spans="1:3">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>178</v>
       </c>
@@ -2465,7 +2469,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="56" spans="1:3">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>179</v>
       </c>
@@ -2473,7 +2477,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="57" spans="1:3">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>180</v>
       </c>
@@ -2481,7 +2485,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="58" spans="1:3">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>181</v>
       </c>
@@ -2489,7 +2493,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="59" spans="1:3">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>182</v>
       </c>
@@ -2497,7 +2501,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="60" spans="1:3">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>183</v>
       </c>
@@ -2505,7 +2509,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="61" spans="1:3">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>184</v>
       </c>
@@ -2513,7 +2517,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="62" spans="1:3">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>185</v>
       </c>
@@ -2521,7 +2525,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="63" spans="1:3">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>186</v>
       </c>
@@ -2529,7 +2533,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="64" spans="1:3">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>187</v>
       </c>
@@ -2537,7 +2541,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="65" spans="1:3">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>188</v>
       </c>
@@ -2545,7 +2549,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="66" spans="1:3">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>189</v>
       </c>
@@ -2553,7 +2557,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="67" spans="1:3">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>46</v>
       </c>
@@ -2567,19 +2571,19 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:DN112"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="53.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="53.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:118">
+    <row r="1" spans="1:118" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>49</v>
       </c>
@@ -2590,7 +2594,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="2" spans="1:118">
+    <row r="2" spans="1:118" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
         <v>125</v>
       </c>
@@ -2598,7 +2602,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="3" spans="1:118">
+    <row r="3" spans="1:118" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>126</v>
       </c>
@@ -2606,7 +2610,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="4" spans="1:118">
+    <row r="4" spans="1:118" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>127</v>
       </c>
@@ -2614,18 +2618,18 @@
         <v>192</v>
       </c>
     </row>
-    <row r="5" spans="1:118">
+    <row r="5" spans="1:118" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>255</v>
       </c>
       <c r="B5" t="s">
-        <v>255</v>
+        <v>357</v>
       </c>
       <c r="C5" t="s">
         <v>312</v>
       </c>
     </row>
-    <row r="6" spans="1:118">
+    <row r="6" spans="1:118" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>256</v>
       </c>
@@ -2637,7 +2641,7 @@
       </c>
       <c r="DN6" s="2"/>
     </row>
-    <row r="7" spans="1:118">
+    <row r="7" spans="1:118" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>257</v>
       </c>
@@ -2648,7 +2652,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="8" spans="1:118">
+    <row r="8" spans="1:118" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>345</v>
       </c>
@@ -2659,7 +2663,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="9" spans="1:118">
+    <row r="9" spans="1:118" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>258</v>
       </c>
@@ -2670,7 +2674,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="10" spans="1:118">
+    <row r="10" spans="1:118" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>259</v>
       </c>
@@ -2681,7 +2685,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="11" spans="1:118">
+    <row r="11" spans="1:118" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>260</v>
       </c>
@@ -2692,7 +2696,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="12" spans="1:118">
+    <row r="12" spans="1:118" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>261</v>
       </c>
@@ -2703,7 +2707,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="13" spans="1:118">
+    <row r="13" spans="1:118" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>262</v>
       </c>
@@ -2714,7 +2718,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="14" spans="1:118">
+    <row r="14" spans="1:118" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>263</v>
       </c>
@@ -2725,7 +2729,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="15" spans="1:118">
+    <row r="15" spans="1:118" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>264</v>
       </c>
@@ -2736,7 +2740,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="16" spans="1:118">
+    <row r="16" spans="1:118" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>265</v>
       </c>
@@ -2747,7 +2751,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="17" spans="1:9">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>266</v>
       </c>
@@ -2758,7 +2762,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="18" spans="1:9">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>2</v>
       </c>
@@ -2769,7 +2773,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="19" spans="1:9">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>267</v>
       </c>
@@ -2780,7 +2784,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="20" spans="1:9">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>268</v>
       </c>
@@ -2791,7 +2795,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="21" spans="1:9">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>269</v>
       </c>
@@ -2802,7 +2806,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="22" spans="1:9">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>270</v>
       </c>
@@ -2813,7 +2817,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="23" spans="1:9">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>271</v>
       </c>
@@ -2824,7 +2828,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="24" spans="1:9">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>272</v>
       </c>
@@ -2835,7 +2839,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="25" spans="1:9">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>273</v>
       </c>
@@ -2846,7 +2850,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="26" spans="1:9">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>274</v>
       </c>
@@ -2857,7 +2861,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="27" spans="1:9">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>128</v>
       </c>
@@ -2868,7 +2872,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="28" spans="1:9">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>129</v>
       </c>
@@ -2879,7 +2883,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="29" spans="1:9">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>275</v>
       </c>
@@ -2890,7 +2894,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="30" spans="1:9">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>150</v>
       </c>
@@ -2902,7 +2906,7 @@
       </c>
       <c r="I30" s="2"/>
     </row>
-    <row r="31" spans="1:9">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>151</v>
       </c>
@@ -2913,7 +2917,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="32" spans="1:9">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>276</v>
       </c>
@@ -2924,7 +2928,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="33" spans="1:3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>132</v>
       </c>
@@ -2935,7 +2939,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="34" spans="1:3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>133</v>
       </c>
@@ -2946,7 +2950,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="35" spans="1:3">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>277</v>
       </c>
@@ -2957,7 +2961,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="36" spans="1:3">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>180</v>
       </c>
@@ -2968,7 +2972,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="37" spans="1:3">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>181</v>
       </c>
@@ -2979,7 +2983,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="38" spans="1:3">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>278</v>
       </c>
@@ -2990,7 +2994,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="39" spans="1:3">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>146</v>
       </c>
@@ -3001,7 +3005,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="40" spans="1:3">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>147</v>
       </c>
@@ -3012,7 +3016,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="41" spans="1:3">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>279</v>
       </c>
@@ -3023,7 +3027,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="42" spans="1:3">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>136</v>
       </c>
@@ -3034,7 +3038,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="43" spans="1:3">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>137</v>
       </c>
@@ -3045,7 +3049,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="44" spans="1:3">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>280</v>
       </c>
@@ -3056,7 +3060,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="45" spans="1:3">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>186</v>
       </c>
@@ -3067,7 +3071,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="46" spans="1:3">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>187</v>
       </c>
@@ -3078,7 +3082,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="47" spans="1:3">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>281</v>
       </c>
@@ -3089,7 +3093,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="48" spans="1:3">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>168</v>
       </c>
@@ -3100,7 +3104,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="49" spans="1:3">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>169</v>
       </c>
@@ -3111,7 +3115,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="50" spans="1:3">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>282</v>
       </c>
@@ -3122,7 +3126,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="51" spans="1:3">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>142</v>
       </c>
@@ -3133,7 +3137,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="52" spans="1:3">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>143</v>
       </c>
@@ -3144,7 +3148,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="53" spans="1:3">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>283</v>
       </c>
@@ -3155,7 +3159,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="54" spans="1:3">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>148</v>
       </c>
@@ -3166,7 +3170,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="55" spans="1:3">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>149</v>
       </c>
@@ -3177,7 +3181,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="56" spans="1:3">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>284</v>
       </c>
@@ -3188,7 +3192,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="57" spans="1:3">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>174</v>
       </c>
@@ -3199,7 +3203,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="58" spans="1:3">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>175</v>
       </c>
@@ -3210,7 +3214,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="59" spans="1:3">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>285</v>
       </c>
@@ -3221,7 +3225,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="60" spans="1:3">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>154</v>
       </c>
@@ -3232,7 +3236,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="61" spans="1:3">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>155</v>
       </c>
@@ -3243,7 +3247,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="62" spans="1:3">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>286</v>
       </c>
@@ -3254,7 +3258,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="63" spans="1:3">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>182</v>
       </c>
@@ -3265,7 +3269,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="64" spans="1:3">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>183</v>
       </c>
@@ -3276,7 +3280,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="65" spans="1:3">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>287</v>
       </c>
@@ -3287,7 +3291,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="66" spans="1:3">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>156</v>
       </c>
@@ -3298,7 +3302,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="67" spans="1:3">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>157</v>
       </c>
@@ -3309,7 +3313,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="68" spans="1:3">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>288</v>
       </c>
@@ -3320,7 +3324,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="69" spans="1:3">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>160</v>
       </c>
@@ -3331,7 +3335,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="70" spans="1:3">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>161</v>
       </c>
@@ -3342,7 +3346,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="71" spans="1:3">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>289</v>
       </c>
@@ -3353,7 +3357,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="72" spans="1:3">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>178</v>
       </c>
@@ -3364,7 +3368,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="73" spans="1:3">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>179</v>
       </c>
@@ -3375,7 +3379,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="74" spans="1:3">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>290</v>
       </c>
@@ -3386,7 +3390,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="75" spans="1:3">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>162</v>
       </c>
@@ -3397,7 +3401,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="76" spans="1:3">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>163</v>
       </c>
@@ -3408,7 +3412,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="77" spans="1:3">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>291</v>
       </c>
@@ -3419,7 +3423,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="78" spans="1:3">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>138</v>
       </c>
@@ -3430,7 +3434,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="79" spans="1:3">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>139</v>
       </c>
@@ -3441,7 +3445,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="80" spans="1:3">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>292</v>
       </c>
@@ -3452,7 +3456,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="81" spans="1:3">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>164</v>
       </c>
@@ -3463,7 +3467,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="82" spans="1:3">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>165</v>
       </c>
@@ -3474,7 +3478,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="83" spans="1:3">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>293</v>
       </c>
@@ -3485,7 +3489,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="84" spans="1:3">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>170</v>
       </c>
@@ -3496,7 +3500,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="85" spans="1:3">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>171</v>
       </c>
@@ -3507,7 +3511,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="86" spans="1:3">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>294</v>
       </c>
@@ -3518,7 +3522,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="87" spans="1:3">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>134</v>
       </c>
@@ -3529,7 +3533,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="88" spans="1:3">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>135</v>
       </c>
@@ -3540,7 +3544,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="89" spans="1:3">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>295</v>
       </c>
@@ -3551,7 +3555,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="90" spans="1:3">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>166</v>
       </c>
@@ -3562,7 +3566,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="91" spans="1:3">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>167</v>
       </c>
@@ -3573,7 +3577,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="92" spans="1:3">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>140</v>
       </c>
@@ -3584,7 +3588,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="93" spans="1:3">
+    <row r="93" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>141</v>
       </c>
@@ -3595,7 +3599,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="94" spans="1:3">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>176</v>
       </c>
@@ -3606,7 +3610,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="95" spans="1:3">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>177</v>
       </c>
@@ -3617,7 +3621,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="96" spans="1:3">
+    <row r="96" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>152</v>
       </c>
@@ -3628,7 +3632,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="97" spans="1:3">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>153</v>
       </c>
@@ -3639,7 +3643,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="98" spans="1:3">
+    <row r="98" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>130</v>
       </c>
@@ -3650,7 +3654,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="99" spans="1:3">
+    <row r="99" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>131</v>
       </c>
@@ -3661,7 +3665,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="100" spans="1:3">
+    <row r="100" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>144</v>
       </c>
@@ -3672,7 +3676,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="101" spans="1:3">
+    <row r="101" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>145</v>
       </c>
@@ -3683,7 +3687,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="102" spans="1:3">
+    <row r="102" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>296</v>
       </c>
@@ -3694,7 +3698,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="103" spans="1:3">
+    <row r="103" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>184</v>
       </c>
@@ -3705,7 +3709,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="104" spans="1:3">
+    <row r="104" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>185</v>
       </c>
@@ -3716,7 +3720,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="105" spans="1:3">
+    <row r="105" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>158</v>
       </c>
@@ -3727,7 +3731,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="106" spans="1:3">
+    <row r="106" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>159</v>
       </c>
@@ -3738,7 +3742,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="107" spans="1:3">
+    <row r="107" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>297</v>
       </c>
@@ -3749,7 +3753,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="108" spans="1:3">
+    <row r="108" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>188</v>
       </c>
@@ -3760,7 +3764,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="109" spans="1:3">
+    <row r="109" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>189</v>
       </c>
@@ -3771,7 +3775,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="110" spans="1:3">
+    <row r="110" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
         <v>172</v>
       </c>
@@ -3782,7 +3786,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="111" spans="1:3">
+    <row r="111" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
         <v>173</v>
       </c>
@@ -3793,7 +3797,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="112" spans="1:3">
+    <row r="112" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
         <v>46</v>
       </c>

</xml_diff>